<commit_message>
Try to fix bugs in the service imports
</commit_message>
<xml_diff>
--- a/vignettes/service_imports.xlsx
+++ b/vignettes/service_imports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johannes Schnebel\Documents\IFW\ifwtrends\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cb9e74139d05168d/IfW/ifwtrends/vignettes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7423E135-2CC6-469F-A82C-7D9FA5AF1173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{7423E135-2CC6-469F-A82C-7D9FA5AF1173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3B1CCCB-7C0E-469A-A1D6-4C4A0B2C2D45}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{49500C68-38B8-4E88-AADE-0525B2BC44ED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{49500C68-38B8-4E88-AADE-0525B2BC44ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
-  <si>
-    <t>#N/A</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>BD IMPORTS - SERVICES CONA</t>
   </si>
@@ -75,10 +72,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -103,7 +101,7 @@
       <tp t="s">
         <v>Name</v>
         <stp/>
-        <stp>{E7064C28-A24F-4A6F-B908-6891E72AD1EC}</stp>
+        <stp>{DAC3FCB6-E3D5-470E-B39A-AD198F51B1E4}</stp>
         <tr r="A1" s="1"/>
       </tp>
     </main>
@@ -408,24 +406,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75B87620-FD6F-4E02-BCC6-81A3B9FC52F1}">
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:R65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
-        <f>_xll.DSGRID("BDEAISTCD"," ","2006-01-01"," ","Q","RowHeader=true;ColHeader=true;DispSeriesDescription=true;YearlyTSFormat=false;QuarterlyTSFormat=true")</f>
+        <f>_xll.DSGRID("BDEAISTCD"," ","2006-01-01","TIME","Q","RowHeader=true;ColHeader=true;DispSeriesDescription=true;YearlyTSFormat=false;QuarterlyTSFormat=true")</f>
         <v>Name</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>38763</v>
       </c>
@@ -433,7 +429,7 @@
         <v>50.668280000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>38852</v>
       </c>
@@ -441,7 +437,7 @@
         <v>50.049799999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>38944</v>
       </c>
@@ -449,7 +445,7 @@
         <v>51.212009999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>39036</v>
       </c>
@@ -457,15 +453,16 @@
         <v>53.047080000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>39128</v>
       </c>
       <c r="B6">
         <v>52.520319999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="R6" s="3"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>39217</v>
       </c>
@@ -473,7 +470,7 @@
         <v>52.554310000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>39309</v>
       </c>
@@ -481,7 +478,7 @@
         <v>54.552370000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>39401</v>
       </c>
@@ -489,7 +486,7 @@
         <v>54.253340000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>39493</v>
       </c>
@@ -497,7 +494,7 @@
         <v>53.86936</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>39583</v>
       </c>
@@ -505,7 +502,7 @@
         <v>55.228670000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>39675</v>
       </c>
@@ -513,7 +510,7 @@
         <v>54.256770000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>39767</v>
       </c>
@@ -521,7 +518,7 @@
         <v>52.999400000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>39859</v>
       </c>
@@ -529,7 +526,7 @@
         <v>49.913919999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>39948</v>
       </c>
@@ -537,7 +534,7 @@
         <v>49.995469999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>40040</v>
       </c>
@@ -545,7 +542,7 @@
         <v>50.022660000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>40132</v>
       </c>
@@ -553,7 +550,7 @@
         <v>48.948810000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>40224</v>
       </c>
@@ -561,7 +558,7 @@
         <v>52.290930000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>40313</v>
       </c>
@@ -569,7 +566,7 @@
         <v>56.171619999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>40405</v>
       </c>
@@ -577,7 +574,7 @@
         <v>55.138579999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>40497</v>
       </c>
@@ -585,7 +582,7 @@
         <v>54.968679999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>40589</v>
       </c>
@@ -593,7 +590,7 @@
         <v>56.29909</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>40678</v>
       </c>
@@ -601,7 +598,7 @@
         <v>57.35248</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>40770</v>
       </c>
@@ -609,7 +606,7 @@
         <v>57.841799999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>40862</v>
       </c>
@@ -617,7 +614,7 @@
         <v>57.597140000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>40954</v>
       </c>
@@ -625,7 +622,7 @@
         <v>60.278300000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>41044</v>
       </c>
@@ -633,7 +630,7 @@
         <v>60.631709999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>41136</v>
       </c>
@@ -641,7 +638,7 @@
         <v>62.167720000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>41228</v>
       </c>
@@ -649,7 +646,7 @@
         <v>60.264710000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>41320</v>
       </c>
@@ -657,7 +654,7 @@
         <v>63.382530000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>41409</v>
       </c>
@@ -665,7 +662,7 @@
         <v>63.899039999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>41501</v>
       </c>
@@ -673,7 +670,7 @@
         <v>63.239800000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>41593</v>
       </c>
@@ -681,7 +678,7 @@
         <v>62.947560000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>41685</v>
       </c>
@@ -689,7 +686,7 @@
         <v>62.83202</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>41774</v>
       </c>
@@ -697,7 +694,7 @@
         <v>63.518450000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>41866</v>
       </c>
@@ -705,7 +702,7 @@
         <v>65.020439999999994</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>41958</v>
       </c>
@@ -713,7 +710,7 @@
         <v>66.175809999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>42050</v>
       </c>
@@ -721,7 +718,7 @@
         <v>66.060280000000006</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>42139</v>
       </c>
@@ -729,7 +726,7 @@
         <v>66.943799999999996</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>42231</v>
       </c>
@@ -737,7 +734,7 @@
         <v>67.460319999999996</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>42323</v>
       </c>
@@ -745,7 +742,7 @@
         <v>70.668180000000007</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>42415</v>
       </c>
@@ -753,7 +750,7 @@
         <v>70.615499999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42505</v>
       </c>
@@ -761,7 +758,7 @@
         <v>71.539829999999995</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>42597</v>
       </c>
@@ -769,7 +766,7 @@
         <v>70.29607</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>42689</v>
       </c>
@@ -777,7 +774,7 @@
         <v>72.756389999999996</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>42781</v>
       </c>
@@ -785,7 +782,7 @@
         <v>74.188680000000005</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>42870</v>
       </c>
@@ -793,7 +790,7 @@
         <v>77.484909999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>42962</v>
       </c>
@@ -801,7 +798,7 @@
         <v>75.364450000000005</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>43054</v>
       </c>
@@ -809,7 +806,7 @@
         <v>77.022750000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>43146</v>
       </c>
@@ -817,7 +814,7 @@
         <v>76.166409999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>43235</v>
       </c>
@@ -825,7 +822,7 @@
         <v>75.54795</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>43327</v>
       </c>
@@ -833,7 +830,7 @@
         <v>77.410139999999998</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>43419</v>
       </c>
@@ -841,7 +838,7 @@
         <v>79.54419</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>43511</v>
       </c>
@@ -849,7 +846,7 @@
         <v>79.855130000000003</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>43600</v>
       </c>
@@ -857,7 +854,7 @@
         <v>80.072609999999997</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>43692</v>
       </c>
@@ -865,7 +862,7 @@
         <v>79.705609999999993</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>43784</v>
       </c>
@@ -873,7 +870,7 @@
         <v>81.82602</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>43876</v>
       </c>
@@ -881,7 +878,7 @@
         <v>79.100290000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>43966</v>
       </c>
@@ -889,7 +886,7 @@
         <v>54.640970000000003</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>44058</v>
       </c>
@@ -897,7 +894,7 @@
         <v>60.050710000000002</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>44150</v>
       </c>
@@ -905,7 +902,7 @@
         <v>57.855559999999997</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>44242</v>
       </c>
@@ -913,34 +910,27 @@
         <v>63.306060000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>44331</v>
       </c>
       <c r="B63">
-        <v>62.551690000000001</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+        <v>63.061399999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>44423</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
-        <v>44515</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="B64" s="2">
+        <v>72.508030000000005</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
+      <c r="B65" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <customProperties>
-    <customPr name="REFI_OFFICE_FUNCTION_DATA" r:id="rId1"/>
-  </customProperties>
 </worksheet>
 </file>
</xml_diff>